<commit_message>
if tts_enable==1: inserted before tts_animation()
</commit_message>
<xml_diff>
--- a/source/Knowledge/Database/RMI_researchers.xlsx
+++ b/source/Knowledge/Database/RMI_researchers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschoi/work/ChatBot/Face_Detect/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschoi/work/ChatBot/FaceBot/source/Knowledge/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C98BEDFA-261B-B344-B5C8-0A485AA776F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82967D40-7260-8D43-BD84-007E29A83B78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="4680" windowWidth="28300" windowHeight="17440" xr2:uid="{BE90FEEF-0071-3141-BA08-DDBFE6223CDC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,6 +244,50 @@
   </si>
   <si>
     <t>ysmin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고미라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>miko</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>miko@kist.re.kr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김익재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영상미디어연구단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drjay@kist.re.kr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drjay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강성철</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의료로봇연구단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kasch@kist.re.kr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kasch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -624,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F99B4F9-49F5-F348-8D5C-56FACE6FD4B9}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="174" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -934,6 +978,66 @@
       </c>
       <c r="F18" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>8302</v>
+      </c>
+      <c r="D19">
+        <v>6323</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20">
+        <v>1347</v>
+      </c>
+      <c r="D20">
+        <v>5766</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>8403</v>
+      </c>
+      <c r="D21">
+        <v>5589</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -951,6 +1055,9 @@
     <hyperlink ref="E11" r:id="rId10" xr:uid="{63054DE8-240E-D240-91BA-B50ADAE4B585}"/>
     <hyperlink ref="E13" r:id="rId11" xr:uid="{E3EA0595-21A8-8949-B2E4-3EFDA648D8AC}"/>
     <hyperlink ref="E12" r:id="rId12" xr:uid="{19BAE2DC-9A57-F64E-94A3-7F78F952C1BF}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{4856AB0E-81C7-794F-9DC4-DEB210D22FA0}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{54B0890A-5768-CA4A-88C3-56A86552D45B}"/>
+    <hyperlink ref="E21" r:id="rId15" xr:uid="{8998BE68-B063-8D4A-8DAD-827D9288604D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Important! save_registered_face in fr_dlib.py fixed
</commit_message>
<xml_diff>
--- a/source/Knowledge/Database/RMI_researchers.xlsx
+++ b/source/Knowledge/Database/RMI_researchers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschoi/work/ChatBot/FaceBot/source/Knowledge/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82967D40-7260-8D43-BD84-007E29A83B78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468346F2-1682-9447-A4FA-4B25762784B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="4680" windowWidth="28300" windowHeight="17440" xr2:uid="{BE90FEEF-0071-3141-BA08-DDBFE6223CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -163,10 +163,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yuh.junku</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bhu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -288,6 +284,10 @@
   </si>
   <si>
     <t>kasch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuh_junku</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F99B4F9-49F5-F348-8D5C-56FACE6FD4B9}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="174" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -697,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -757,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -777,7 +777,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -797,7 +797,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -817,7 +817,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -837,7 +837,7 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -857,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -877,7 +877,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -897,7 +897,7 @@
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -917,7 +917,7 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -937,52 +937,52 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
         <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
         <v>47</v>
-      </c>
-      <c r="F15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
         <v>49</v>
-      </c>
-      <c r="F16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
         <v>51</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
         <v>53</v>
-      </c>
-      <c r="F18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -994,18 +994,18 @@
         <v>6323</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
       </c>
       <c r="C20">
         <v>1347</v>
@@ -1014,18 +1014,18 @@
         <v>5766</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
         <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
       </c>
       <c r="C21">
         <v>8403</v>
@@ -1034,10 +1034,10 @@
         <v>5589</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
         <v>64</v>
-      </c>
-      <c r="F21" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>